<commit_message>
CI: actualizar DB/Stock V/reportes + índices (commit times)
</commit_message>
<xml_diff>
--- a/_db/Disco_Pro_DB_HOJA1.xlsx
+++ b/_db/Disco_Pro_DB_HOJA1.xlsx
@@ -1549,7 +1549,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -1559,7 +1559,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114">
@@ -4109,7 +4109,7 @@
         </is>
       </c>
       <c r="B368" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="369">
@@ -4119,7 +4119,7 @@
         </is>
       </c>
       <c r="B369" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="370">
@@ -7749,7 +7749,7 @@
         </is>
       </c>
       <c r="B732" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="733">
@@ -7759,7 +7759,7 @@
         </is>
       </c>
       <c r="B733" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="734">
@@ -7769,7 +7769,7 @@
         </is>
       </c>
       <c r="B734" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="735">
@@ -7779,7 +7779,7 @@
         </is>
       </c>
       <c r="B735" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="736">
@@ -7809,7 +7809,7 @@
         </is>
       </c>
       <c r="B738" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="739">
@@ -7819,7 +7819,7 @@
         </is>
       </c>
       <c r="B739" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="740">
@@ -7829,7 +7829,7 @@
         </is>
       </c>
       <c r="B740" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="741">
@@ -7839,7 +7839,7 @@
         </is>
       </c>
       <c r="B741" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="742">
@@ -7849,7 +7849,7 @@
         </is>
       </c>
       <c r="B742" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="743">
@@ -7859,7 +7859,7 @@
         </is>
       </c>
       <c r="B743" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="744">
@@ -7889,7 +7889,7 @@
         </is>
       </c>
       <c r="B746" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="747">
@@ -7899,7 +7899,7 @@
         </is>
       </c>
       <c r="B747" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="748">
@@ -7969,7 +7969,7 @@
         </is>
       </c>
       <c r="B754" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="755">
@@ -7979,7 +7979,7 @@
         </is>
       </c>
       <c r="B755" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="756">
@@ -8009,7 +8009,7 @@
         </is>
       </c>
       <c r="B758" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="759">
@@ -8019,7 +8019,7 @@
         </is>
       </c>
       <c r="B759" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="760">
@@ -8069,7 +8069,7 @@
         </is>
       </c>
       <c r="B764" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="765">
@@ -8079,7 +8079,7 @@
         </is>
       </c>
       <c r="B765" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="766">
@@ -8089,7 +8089,7 @@
         </is>
       </c>
       <c r="B766" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="767">
@@ -8099,7 +8099,7 @@
         </is>
       </c>
       <c r="B767" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="768">
@@ -8129,7 +8129,7 @@
         </is>
       </c>
       <c r="B770" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="771">
@@ -8139,7 +8139,7 @@
         </is>
       </c>
       <c r="B771" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="772">
@@ -8149,7 +8149,7 @@
         </is>
       </c>
       <c r="B772" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="773">
@@ -8159,7 +8159,7 @@
         </is>
       </c>
       <c r="B773" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="774">
@@ -8209,7 +8209,7 @@
         </is>
       </c>
       <c r="B778" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="779">
@@ -8219,7 +8219,7 @@
         </is>
       </c>
       <c r="B779" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="780">
@@ -8309,7 +8309,7 @@
         </is>
       </c>
       <c r="B788" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="789">
@@ -8319,7 +8319,7 @@
         </is>
       </c>
       <c r="B789" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="790">
@@ -8329,7 +8329,7 @@
         </is>
       </c>
       <c r="B790" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="791">
@@ -8339,7 +8339,7 @@
         </is>
       </c>
       <c r="B791" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="792">
@@ -8389,7 +8389,7 @@
         </is>
       </c>
       <c r="B796" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="797">
@@ -8399,7 +8399,7 @@
         </is>
       </c>
       <c r="B797" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="798">
@@ -8409,7 +8409,7 @@
         </is>
       </c>
       <c r="B798" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="799">
@@ -8419,7 +8419,7 @@
         </is>
       </c>
       <c r="B799" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="800">
@@ -8429,7 +8429,7 @@
         </is>
       </c>
       <c r="B800" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="801">
@@ -8439,7 +8439,7 @@
         </is>
       </c>
       <c r="B801" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="802">
@@ -13789,7 +13789,7 @@
         </is>
       </c>
       <c r="B1336" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1337">

</xml_diff>